<commit_message>
Coal High Cost runs completed
</commit_message>
<xml_diff>
--- a/india_REV_input/Scenarios_Cost_Master_v3.xlsx
+++ b/india_REV_input/Scenarios_Cost_Master_v3.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akjohnson\Desktop\Ranjit\renewable_energy_value\india_REV_input\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-4560" yWindow="-21260" windowWidth="32360" windowHeight="18340"/>
+    <workbookView xWindow="-4560" yWindow="-21255" windowWidth="32355" windowHeight="18345" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="REvalue_input_csv" sheetId="11" r:id="rId1"/>
@@ -18,13 +23,13 @@
     <sheet name="scenarios" sheetId="13" r:id="rId9"/>
     <sheet name="run_times" sheetId="12" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -37,7 +42,7 @@
     <author>Ranjit Deshmukh</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0">
+    <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -61,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D6" authorId="1">
+    <comment ref="D6" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -97,7 +102,7 @@
     <author>Ranjit</author>
   </authors>
   <commentList>
-    <comment ref="AC5" authorId="0">
+    <comment ref="AC5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -122,7 +127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="1">
+    <comment ref="B6" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -147,7 +152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A8" authorId="1">
+    <comment ref="A8" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -171,7 +176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B16" authorId="1">
+    <comment ref="B16" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -196,7 +201,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="1">
+    <comment ref="B18" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -220,7 +225,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D34" authorId="1">
+    <comment ref="D34" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -245,7 +250,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B37" authorId="1">
+    <comment ref="B37" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -269,7 +274,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D37" authorId="1">
+    <comment ref="D37" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -303,7 +308,7 @@
     <author>Ranjit</author>
   </authors>
   <commentList>
-    <comment ref="B22" authorId="0">
+    <comment ref="B22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -328,7 +333,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C22" authorId="0">
+    <comment ref="C22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -352,7 +357,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="0">
+    <comment ref="D22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -377,7 +382,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E22" authorId="0">
+    <comment ref="E22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -402,7 +407,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E34" authorId="0">
+    <comment ref="E34" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -426,7 +431,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B61" authorId="0">
+    <comment ref="B61" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1771,9 +1776,6 @@
     <t>USD/kW (2018)</t>
   </si>
   <si>
-    <t>Prayas analysis forthcoming report - Rs 7 crore per MW from CEA data + FGD cost of Rs 40 lakhs per MW from http://www.cercind.gov.in/2018/orders/104.pdf</t>
-  </si>
-  <si>
     <t xml:space="preserve">Coal High Cost (USD/GJ) </t>
   </si>
   <si>
@@ -1787,6 +1789,9 @@
   </si>
   <si>
     <t>coalHC_wind30LC_solar30LC</t>
+  </si>
+  <si>
+    <t>Prayas analysis forthcoming report - Rs 7.5 crore per MW from CEA data + FGD cost of Rs 50 lakhs per MW from http://www.cercind.gov.in/2018/orders/104.pdf</t>
   </si>
 </sst>
 </file>
@@ -1794,12 +1799,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="6">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
-    <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -1899,7 +1904,7 @@
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1912,28 +1917,28 @@
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2229,7 +2234,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2239,36 +2244,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
       <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="14" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="14" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>228</v>
       </c>
@@ -2348,10 +2353,10 @@
         <v>427</v>
       </c>
       <c r="AA1" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>247</v>
       </c>
@@ -2455,7 +2460,7 @@
         <v>ClcC70mB30B50lc</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>249</v>
       </c>
@@ -2556,7 +2561,7 @@
         <v>ClcC70mB30B50lc</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>418</v>
       </c>
@@ -2657,7 +2662,7 @@
         <v>ClcC70mB30</v>
       </c>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>250</v>
       </c>
@@ -2758,7 +2763,7 @@
         <v>coallcB30</v>
       </c>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>251</v>
       </c>
@@ -2859,7 +2864,7 @@
         <v>coallcB30</v>
       </c>
     </row>
-    <row r="7" spans="1:27">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>252</v>
       </c>
@@ -2960,7 +2965,7 @@
         <v>W80_S0d</v>
       </c>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>253</v>
       </c>
@@ -3061,7 +3066,7 @@
         <v>coallcB50lc</v>
       </c>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>254</v>
       </c>
@@ -3141,7 +3146,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>258</v>
       </c>
@@ -3242,7 +3247,7 @@
         <v>Clc</v>
       </c>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>259</v>
       </c>
@@ -3343,7 +3348,7 @@
         <v>coallc</v>
       </c>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>260</v>
       </c>
@@ -3423,7 +3428,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>262</v>
       </c>
@@ -3524,7 +3529,7 @@
         <v>C70m</v>
       </c>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>263</v>
       </c>
@@ -3604,7 +3609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>265</v>
       </c>
@@ -3705,7 +3710,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:27">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>266</v>
       </c>
@@ -3785,7 +3790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:26">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>268</v>
       </c>
@@ -3886,7 +3891,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>269</v>
       </c>
@@ -3966,7 +3971,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>271</v>
       </c>
@@ -4067,7 +4072,7 @@
         <v>B30</v>
       </c>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>272</v>
       </c>
@@ -4168,7 +4173,7 @@
         <v>bat30</v>
       </c>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>420</v>
       </c>
@@ -4248,7 +4253,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>421</v>
       </c>
@@ -4328,7 +4333,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>422</v>
       </c>
@@ -4429,7 +4434,7 @@
         <v>B50lc</v>
       </c>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>423</v>
       </c>
@@ -4530,7 +4535,7 @@
         <v>batteryLC50</v>
       </c>
     </row>
-    <row r="25" spans="1:26">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
         <v>273</v>
       </c>
@@ -4610,7 +4615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:26">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>275</v>
       </c>
@@ -4690,7 +4695,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="27" spans="1:26">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>277</v>
       </c>
@@ -4791,7 +4796,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:26">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>278</v>
       </c>
@@ -4892,7 +4897,7 @@
         <v>windLC0</v>
       </c>
     </row>
-    <row r="29" spans="1:26">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
         <v>279</v>
       </c>
@@ -4972,7 +4977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:26">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>280</v>
       </c>
@@ -5052,7 +5057,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="31" spans="1:26">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>281</v>
       </c>
@@ -5153,7 +5158,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:26">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>282</v>
       </c>
@@ -5254,7 +5259,7 @@
         <v>solarLC0</v>
       </c>
     </row>
-    <row r="33" spans="1:26">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
         <v>283</v>
       </c>
@@ -5334,7 +5339,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:26">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>285</v>
       </c>
@@ -5435,7 +5440,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:26">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>286</v>
       </c>
@@ -5536,7 +5541,7 @@
         <v>W80</v>
       </c>
     </row>
-    <row r="36" spans="1:26">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
         <v>287</v>
       </c>
@@ -5616,7 +5621,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="37" spans="1:26">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>292</v>
       </c>
@@ -5717,7 +5722,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:26">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>293</v>
       </c>
@@ -5818,7 +5823,7 @@
         <v>S0d</v>
       </c>
     </row>
-    <row r="39" spans="1:26">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
         <v>294</v>
       </c>
@@ -5896,7 +5901,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="40" spans="1:26">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>295</v>
       </c>
@@ -5997,7 +6002,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:26">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
         <v>296</v>
       </c>
@@ -6077,7 +6082,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="42" spans="1:26">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>300</v>
       </c>
@@ -6178,7 +6183,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:26">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
         <v>301</v>
       </c>
@@ -6258,7 +6263,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="44" spans="1:26">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>304</v>
       </c>
@@ -6335,7 +6340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:26">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>305</v>
       </c>
@@ -6456,13 +6461,13 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="36.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.83203125" customWidth="1"/>
+    <col min="6" max="6" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>317</v>
       </c>
@@ -6473,7 +6478,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>314</v>
       </c>
@@ -6490,7 +6495,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>308</v>
       </c>
@@ -6515,7 +6520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>308</v>
       </c>
@@ -6540,7 +6545,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>308</v>
       </c>
@@ -6559,7 +6564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>308</v>
       </c>
@@ -6603,14 +6608,14 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="str">
         <f>REvalue_input_csv!C1</f>
         <v>base</v>
@@ -6624,7 +6629,7 @@
         <v>coal_55mingen</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="str">
         <f>REvalue_input_csv!C2</f>
         <v>ClcC70m</v>
@@ -6638,7 +6643,7 @@
         <v>ClcC55m</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>414</v>
       </c>
@@ -6646,7 +6651,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>415</v>
       </c>
@@ -6654,7 +6659,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>411</v>
       </c>
@@ -6662,7 +6667,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>412</v>
       </c>
@@ -6670,7 +6675,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>413</v>
       </c>
@@ -6689,39 +6694,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL73"/>
   <sheetViews>
-    <sheetView topLeftCell="K15" workbookViewId="0">
-      <selection activeCell="R55" sqref="R55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T53" sqref="T53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.5" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" customWidth="1"/>
-    <col min="7" max="7" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14" customWidth="1"/>
-    <col min="20" max="20" width="11.5" customWidth="1"/>
-    <col min="21" max="21" width="24.5" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" customWidth="1"/>
+    <col min="21" max="21" width="24.42578125" customWidth="1"/>
     <col min="22" max="22" width="12" customWidth="1"/>
-    <col min="23" max="23" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.33203125" customWidth="1"/>
-    <col min="25" max="25" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.5" customWidth="1"/>
-    <col min="27" max="27" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.28515625" customWidth="1"/>
+    <col min="25" max="25" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.42578125" customWidth="1"/>
+    <col min="27" max="27" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="28" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="28.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -6735,7 +6740,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:38">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>35</v>
       </c>
@@ -6743,7 +6748,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>34</v>
       </c>
@@ -6790,7 +6795,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>54</v>
       </c>
@@ -6812,7 +6817,7 @@
       </c>
       <c r="U4" s="5">
         <f>'Data and sources'!D19</f>
-        <v>1140</v>
+        <v>1230</v>
       </c>
       <c r="V4" t="s">
         <v>172</v>
@@ -6874,7 +6879,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -6948,7 +6953,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -6998,7 +7003,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -7029,7 +7034,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:38">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -7040,7 +7045,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="9" spans="1:38">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -7096,7 +7101,7 @@
         <v>coallcB50lc</v>
       </c>
     </row>
-    <row r="10" spans="1:38">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -7141,7 +7146,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:38">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -7186,7 +7191,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="12" spans="1:38">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>96</v>
       </c>
@@ -7231,7 +7236,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="13" spans="1:38">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -7279,7 +7284,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="14" spans="1:38">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -7337,15 +7342,15 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:38">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B15">
         <v>3.9</v>
       </c>
       <c r="C15" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="R15" t="s">
         <v>189</v>
@@ -7395,7 +7400,7 @@
         <v>8.5810517220665614E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:38">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -7406,7 +7411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:29">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -7465,7 +7470,7 @@
         <v>678.26769230769241</v>
       </c>
     </row>
-    <row r="18" spans="1:29">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>163</v>
       </c>
@@ -7524,7 +7529,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:29">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>165</v>
       </c>
@@ -7580,7 +7585,7 @@
         <v>65.002501490990369</v>
       </c>
     </row>
-    <row r="20" spans="1:29">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -7639,7 +7644,7 @@
         <v>126.97417171717171</v>
       </c>
     </row>
-    <row r="21" spans="1:29">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -7651,7 +7656,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:29">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -7666,7 +7671,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:29">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -7728,7 +7733,7 @@
         <v>775.16307692307703</v>
       </c>
     </row>
-    <row r="24" spans="1:29">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>133</v>
       </c>
@@ -7787,7 +7792,7 @@
         <v>77.517144561131843</v>
       </c>
     </row>
-    <row r="25" spans="1:29">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>52</v>
       </c>
@@ -7845,7 +7850,7 @@
         <v>84.936820512820518</v>
       </c>
     </row>
-    <row r="26" spans="1:29">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -7856,12 +7861,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:29">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="R27" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:29">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -7877,7 +7882,7 @@
       </c>
       <c r="T28" s="5">
         <f t="shared" ref="T28:AA28" si="10">INDEX($T$4:$U$5, MATCH(T10,$T$4:$T$5),2)</f>
-        <v>1140</v>
+        <v>1230</v>
       </c>
       <c r="U28" s="5">
         <f t="shared" si="10"/>
@@ -7916,7 +7921,7 @@
         <v>976.42784318082204</v>
       </c>
     </row>
-    <row r="29" spans="1:29">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>16</v>
       </c>
@@ -7971,7 +7976,7 @@
         <v>2.6153846153846154</v>
       </c>
     </row>
-    <row r="30" spans="1:29">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>1</v>
       </c>
@@ -8002,7 +8007,7 @@
       </c>
       <c r="T30" s="5">
         <f t="shared" si="12"/>
-        <v>139.92398963155881</v>
+        <v>147.64693618141871</v>
       </c>
       <c r="U30" s="5">
         <f t="shared" si="12"/>
@@ -8041,7 +8046,7 @@
         <v>125.88777825200532</v>
       </c>
     </row>
-    <row r="31" spans="1:29">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -8120,7 +8125,7 @@
         <v>32.466607822649564</v>
       </c>
     </row>
-    <row r="32" spans="1:29">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -8152,7 +8157,7 @@
         <v>2736.5</v>
       </c>
     </row>
-    <row r="33" spans="1:29">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -8188,7 +8193,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="34" spans="1:29">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -8261,7 +8266,7 @@
         <v>3.3984353954038309E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:29">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>74</v>
       </c>
@@ -8292,7 +8297,7 @@
       </c>
       <c r="T35" s="2">
         <f t="shared" si="16"/>
-        <v>0.18251009215426989</v>
+        <v>0.2050960069674089</v>
       </c>
       <c r="U35" s="2">
         <f t="shared" si="16"/>
@@ -8331,7 +8336,7 @@
         <v>0.10523612453151106</v>
       </c>
     </row>
-    <row r="36" spans="1:29">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>166</v>
       </c>
@@ -8384,7 +8389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:29">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -8401,7 +8406,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:29">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -8421,7 +8426,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="39" spans="1:29">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -8444,7 +8449,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="40" spans="1:29">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -8515,7 +8520,7 @@
         <v>65.002501490990369</v>
       </c>
     </row>
-    <row r="41" spans="1:29">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -8586,7 +8591,7 @@
         <v>1177.2962457334145</v>
       </c>
     </row>
-    <row r="42" spans="1:29">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -8656,7 +8661,7 @@
         <v>77.517144561131843</v>
       </c>
     </row>
-    <row r="43" spans="1:29">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -8723,7 +8728,7 @@
         <v>821.56369225343963</v>
       </c>
     </row>
-    <row r="44" spans="1:29">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>23</v>
       </c>
@@ -8751,7 +8756,7 @@
       </c>
       <c r="T44" s="5">
         <f t="shared" si="22"/>
-        <v>139.92398963155881</v>
+        <v>147.64693618141871</v>
       </c>
       <c r="U44" s="5">
         <f t="shared" si="22"/>
@@ -8790,7 +8795,7 @@
         <v>125.88777825200532</v>
       </c>
     </row>
-    <row r="45" spans="1:29">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>24</v>
       </c>
@@ -8818,7 +8823,7 @@
       </c>
       <c r="T45" s="5">
         <f t="shared" si="23"/>
-        <v>542.03413077339212</v>
+        <v>549.75707732325202</v>
       </c>
       <c r="U45" s="5">
         <f t="shared" si="23"/>
@@ -8857,7 +8862,7 @@
         <v>410.29526277841552</v>
       </c>
     </row>
-    <row r="46" spans="1:29">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -8874,7 +8879,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="47" spans="1:29">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
       <c r="Q47" s="20" t="s">
         <v>430</v>
       </c>
@@ -8882,7 +8887,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="48" spans="1:29">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -8951,7 +8956,7 @@
         <v>coallcB50lc</v>
       </c>
     </row>
-    <row r="49" spans="1:29">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>18</v>
       </c>
@@ -9018,7 +9023,7 @@
         <v>678.26769230769241</v>
       </c>
     </row>
-    <row r="50" spans="1:29" ht="15">
+    <row r="50" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>19</v>
       </c>
@@ -9085,7 +9090,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="51" spans="1:29">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>20</v>
       </c>
@@ -9152,7 +9157,7 @@
         <v>775.16307692307703</v>
       </c>
     </row>
-    <row r="52" spans="1:29">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>39</v>
       </c>
@@ -9234,7 +9239,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:29">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>32</v>
       </c>
@@ -9271,7 +9276,7 @@
       </c>
       <c r="T53" s="5">
         <f t="shared" si="29"/>
-        <v>1140</v>
+        <v>1230</v>
       </c>
       <c r="U53" s="5">
         <f t="shared" si="29"/>
@@ -9310,7 +9315,7 @@
         <v>976.42784318082204</v>
       </c>
     </row>
-    <row r="54" spans="1:29">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>37</v>
       </c>
@@ -9392,7 +9397,7 @@
         <v>42.1</v>
       </c>
     </row>
-    <row r="55" spans="1:29">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>190</v>
       </c>
@@ -9470,7 +9475,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="56" spans="1:29">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>191</v>
       </c>
@@ -9529,7 +9534,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:29">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B57" s="12"/>
       <c r="Q57" t="s">
         <v>203</v>
@@ -9582,7 +9587,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="58" spans="1:29">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B58" s="12"/>
       <c r="Q58" t="s">
         <v>204</v>
@@ -9635,7 +9640,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:29">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>149</v>
       </c>
@@ -9690,7 +9695,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="60" spans="1:29">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>147</v>
       </c>
@@ -9745,7 +9750,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:29">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>0</v>
       </c>
@@ -9762,7 +9767,7 @@
         <v>125.88777825200532</v>
       </c>
     </row>
-    <row r="62" spans="1:29">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>8760</v>
       </c>
@@ -9779,7 +9784,7 @@
         <v>410.29526277841552</v>
       </c>
     </row>
-    <row r="63" spans="1:29">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>148</v>
       </c>
@@ -9796,12 +9801,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>159</v>
       </c>
@@ -9809,7 +9814,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>432</v>
       </c>
@@ -9820,7 +9825,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>433</v>
       </c>
@@ -9831,7 +9836,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>435</v>
       </c>
@@ -9842,7 +9847,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>153</v>
       </c>
@@ -9855,7 +9860,7 @@
         <v>44.890647132724027</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>155</v>
       </c>
@@ -9868,7 +9873,7 @@
         <v>2.917892063627062</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>434</v>
       </c>
@@ -9899,12 +9904,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>'Screening curves'!Q34</f>
         <v>parameter</v>
@@ -9930,7 +9935,7 @@
         <v>coallcW30lcS30lc</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>'Screening curves'!R34</f>
         <v>gas_ct</v>
@@ -9956,7 +9961,7 @@
         <v>3.3984353954038309E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>'Screening curves'!R35</f>
         <v>gas_ccgt</v>
@@ -9967,7 +9972,7 @@
       </c>
       <c r="C3" s="2">
         <f>'Screening curves'!T35</f>
-        <v>0.18251009215426989</v>
+        <v>0.2050960069674089</v>
       </c>
       <c r="D3" s="2">
         <f>'Screening curves'!W35</f>
@@ -9982,7 +9987,7 @@
         <v>0.10523612453151106</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>'Screening curves'!R36</f>
         <v>coal</v>
@@ -10008,7 +10013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>'Screening curves'!R18</f>
         <v>gas_price</v>
@@ -10034,7 +10039,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>'Screening curves'!R17</f>
         <v>cap_cost_ct</v>
@@ -10060,7 +10065,7 @@
         <v>678.26769230769241</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>'Screening curves'!R23</f>
         <v>cap_cost_ccgt</v>
@@ -10086,7 +10091,7 @@
         <v>775.16307692307703</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>'Screening curves'!R28</f>
         <v>cap_cost_coal</v>
@@ -10097,7 +10102,7 @@
       </c>
       <c r="C8" s="5">
         <f>'Screening curves'!T28</f>
-        <v>1140</v>
+        <v>1230</v>
       </c>
       <c r="D8" s="5">
         <f>'Screening curves'!W28</f>
@@ -10130,13 +10135,13 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>'Screening curves'!Q39</f>
         <v>hour</v>
@@ -10154,7 +10159,7 @@
         <v>coalhc</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>'Screening curves'!Q40</f>
         <v>0</v>
@@ -10172,7 +10177,7 @@
         <v>65.002501490990369</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>'Screening curves'!Q41</f>
         <v>8760</v>
@@ -10190,7 +10195,7 @@
         <v>1177.2962457334145</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>'Screening curves'!Q42</f>
         <v>0</v>
@@ -10208,7 +10213,7 @@
         <v>77.517144561131843</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>'Screening curves'!Q43</f>
         <v>8760</v>
@@ -10226,7 +10231,7 @@
         <v>821.56369225343963</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>'Screening curves'!Q44</f>
         <v>0</v>
@@ -10241,10 +10246,10 @@
       </c>
       <c r="D6" s="5">
         <f>'Screening curves'!T44</f>
-        <v>139.92398963155881</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>147.64693618141871</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>'Screening curves'!Q45</f>
         <v>8760</v>
@@ -10259,7 +10264,7 @@
       </c>
       <c r="D7" s="5">
         <f>'Screening curves'!T45</f>
-        <v>542.03413077339212</v>
+        <v>549.75707732325202</v>
       </c>
     </row>
   </sheetData>
@@ -10280,20 +10285,20 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>'Screening curves'!Q48</f>
         <v>cost_type</v>
@@ -10347,7 +10352,7 @@
         <v>coallcB50lc</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>'Screening curves'!Q49</f>
         <v>capital</v>
@@ -10401,7 +10406,7 @@
         <v>678.26769230769241</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>'Screening curves'!Q50</f>
         <v>om</v>
@@ -10455,7 +10460,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>'Screening curves'!Q51</f>
         <v>capital</v>
@@ -10509,7 +10514,7 @@
         <v>775.16307692307703</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>'Screening curves'!Q52</f>
         <v>om</v>
@@ -10563,7 +10568,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>'Screening curves'!Q53</f>
         <v>capital</v>
@@ -10578,7 +10583,7 @@
       </c>
       <c r="D6" s="5">
         <f>'Screening curves'!T53</f>
-        <v>1140</v>
+        <v>1230</v>
       </c>
       <c r="E6" s="5">
         <f>'Screening curves'!U53</f>
@@ -10617,7 +10622,7 @@
         <v>976.42784318082204</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>'Screening curves'!Q54</f>
         <v>om</v>
@@ -10671,7 +10676,7 @@
         <v>42.1</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>'Screening curves'!Q55</f>
         <v>capital</v>
@@ -10725,7 +10730,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>'Screening curves'!Q56</f>
         <v>om</v>
@@ -10779,7 +10784,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>'Screening curves'!Q57</f>
         <v>capital</v>
@@ -10833,7 +10838,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>'Screening curves'!Q58</f>
         <v>om</v>
@@ -10887,7 +10892,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>'Screening curves'!Q59</f>
         <v>capital</v>
@@ -10941,7 +10946,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>'Screening curves'!Q60</f>
         <v>om</v>
@@ -11009,21 +11014,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
@@ -11046,12 +11051,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>115</v>
       </c>
@@ -11071,7 +11076,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>125</v>
       </c>
@@ -11096,7 +11101,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>85</v>
       </c>
@@ -11119,7 +11124,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>125</v>
       </c>
@@ -11148,7 +11153,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>97</v>
       </c>
@@ -11168,7 +11173,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>108</v>
       </c>
@@ -11192,7 +11197,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>111</v>
       </c>
@@ -11216,7 +11221,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>102</v>
       </c>
@@ -11236,7 +11241,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>108</v>
       </c>
@@ -11260,7 +11265,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>114</v>
       </c>
@@ -11284,7 +11289,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>97</v>
       </c>
@@ -11300,7 +11305,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>108</v>
       </c>
@@ -11318,7 +11323,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>114</v>
       </c>
@@ -11336,7 +11341,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>437</v>
       </c>
@@ -11350,27 +11355,26 @@
         <v>436</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>437</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="14">
-        <f>1077 + 63</f>
-        <v>1140</v>
+        <v>1230</v>
       </c>
       <c r="E19" s="5"/>
       <c r="H19" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>129</v>
       </c>
@@ -11390,7 +11394,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>116</v>
       </c>
@@ -11416,7 +11420,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>130</v>
       </c>
@@ -11438,7 +11442,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>131</v>
       </c>
@@ -11460,7 +11464,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>82</v>
       </c>
@@ -11480,7 +11484,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>88</v>
       </c>
@@ -11497,7 +11501,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>118</v>
       </c>
@@ -11520,7 +11524,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>119</v>
       </c>
@@ -11543,7 +11547,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>122</v>
       </c>
@@ -11572,7 +11576,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>123</v>
       </c>
@@ -11601,12 +11605,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>71</v>
       </c>
@@ -11617,7 +11621,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>71</v>
       </c>
@@ -11631,7 +11635,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>71</v>
       </c>
@@ -11651,7 +11655,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>83</v>
       </c>
@@ -11668,7 +11672,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>95</v>
       </c>
@@ -11689,7 +11693,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>83</v>
       </c>
@@ -11709,7 +11713,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>95</v>
       </c>
@@ -11730,17 +11734,17 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>136</v>
       </c>
@@ -11751,7 +11755,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B47" s="8">
         <v>0.108</v>
       </c>
@@ -11759,12 +11763,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>141</v>
       </c>
@@ -11775,7 +11779,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>8.5</v>
       </c>
@@ -11783,7 +11787,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" s="7">
         <v>10</v>
       </c>
@@ -11791,7 +11795,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>5.5</v>
       </c>
@@ -11799,17 +11803,17 @@
         <v>145</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>150</v>
       </c>
@@ -11820,7 +11824,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>151</v>
       </c>
@@ -11833,7 +11837,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>152</v>
       </c>
@@ -11845,7 +11849,7 @@
       </c>
       <c r="D61" s="17"/>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>162</v>
       </c>
@@ -11859,7 +11863,7 @@
       </c>
       <c r="D62" s="17"/>
     </row>
-    <row r="63" spans="1:4" ht="15">
+    <row r="63" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>17</v>
       </c>
@@ -11871,7 +11875,7 @@
       </c>
       <c r="D63" s="18"/>
     </row>
-    <row r="64" spans="1:4" ht="15">
+    <row r="64" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>156</v>
       </c>
@@ -11883,7 +11887,7 @@
       </c>
       <c r="D64" s="19"/>
     </row>
-    <row r="65" spans="1:4" ht="15">
+    <row r="65" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>19</v>
       </c>
@@ -11897,7 +11901,7 @@
       </c>
       <c r="D65" s="9"/>
     </row>
-    <row r="66" spans="1:4" ht="15">
+    <row r="66" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>157</v>
       </c>
@@ -11909,7 +11913,7 @@
       </c>
       <c r="D66" s="16"/>
     </row>
-    <row r="67" spans="1:4" ht="15">
+    <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>158</v>
       </c>
@@ -11921,7 +11925,7 @@
       </c>
       <c r="D67" s="16"/>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>154</v>
       </c>
@@ -11935,7 +11939,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>153</v>
       </c>
@@ -11949,7 +11953,7 @@
       </c>
       <c r="D69" s="4"/>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>155</v>
       </c>
@@ -11983,40 +11987,40 @@
       <selection activeCell="B14" sqref="B14:B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="30" customHeight="1">
+    <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
         <v>107</v>
       </c>
@@ -12051,7 +12055,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2008</v>
       </c>
@@ -12063,7 +12067,7 @@
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2009</v>
       </c>
@@ -12078,7 +12082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2010</v>
       </c>
@@ -12097,7 +12101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2011</v>
       </c>
@@ -12120,7 +12124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2012</v>
       </c>
@@ -12147,7 +12151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2013</v>
       </c>
@@ -12178,7 +12182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2014</v>
       </c>
@@ -12213,7 +12217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2015</v>
       </c>
@@ -12252,7 +12256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2016</v>
       </c>
@@ -12295,7 +12299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2017</v>
       </c>
@@ -12342,17 +12346,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="28">
+    <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="13" t="s">
         <v>107</v>
       </c>
@@ -12387,7 +12391,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2008</v>
       </c>
@@ -12399,7 +12403,7 @@
       </c>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2009</v>
       </c>
@@ -12414,7 +12418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2010</v>
       </c>
@@ -12433,7 +12437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2011</v>
       </c>
@@ -12456,7 +12460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2012</v>
       </c>
@@ -12483,7 +12487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2013</v>
       </c>
@@ -12514,7 +12518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2014</v>
       </c>
@@ -12549,7 +12553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2015</v>
       </c>
@@ -12588,7 +12592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2016</v>
       </c>
@@ -12631,7 +12635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2017</v>
       </c>
@@ -12696,25 +12700,25 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" customWidth="1"/>
-    <col min="7" max="7" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5" customWidth="1"/>
-    <col min="9" max="9" width="32.83203125" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
+    <col min="9" max="9" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>408</v>
       </c>
@@ -12743,7 +12747,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>400</v>
       </c>
@@ -12754,7 +12758,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>200</v>
       </c>
@@ -12762,7 +12766,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>200</v>
       </c>
@@ -12770,7 +12774,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>200</v>
       </c>
@@ -12778,7 +12782,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>200</v>
       </c>
@@ -12786,7 +12790,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>200</v>
       </c>
@@ -12794,7 +12798,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>300</v>
       </c>
@@ -12802,7 +12806,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>300</v>
       </c>
@@ -12810,7 +12814,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>300</v>
       </c>
@@ -12818,7 +12822,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>300</v>
       </c>
@@ -12826,7 +12830,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>300</v>
       </c>
@@ -12834,7 +12838,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>400</v>
       </c>
@@ -12842,7 +12846,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>400</v>
       </c>
@@ -12850,7 +12854,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>400</v>
       </c>
@@ -12858,7 +12862,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>400</v>
       </c>
@@ -12866,7 +12870,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>400</v>
       </c>
@@ -12874,12 +12878,12 @@
         <v>394</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>392</v>
       </c>
@@ -12887,7 +12891,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D24" s="7" t="s">
         <v>390</v>
       </c>
@@ -12895,7 +12899,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D25" s="7" t="s">
         <v>388</v>
       </c>
@@ -12903,13 +12907,13 @@
         <v>387</v>
       </c>
       <c r="H25" t="s">
+        <v>440</v>
+      </c>
+      <c r="I25" t="s">
         <v>441</v>
       </c>
-      <c r="I25" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E26" s="7" t="s">
         <v>386</v>
       </c>
@@ -12920,7 +12924,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
         <v>384</v>
       </c>
@@ -12931,7 +12935,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
         <v>382</v>
       </c>
@@ -12942,7 +12946,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
         <v>380</v>
       </c>
@@ -12953,7 +12957,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F30" t="s">
         <v>378</v>
       </c>
@@ -12964,7 +12968,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D31" s="7" t="s">
         <v>375</v>
       </c>
@@ -12978,7 +12982,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D32" s="7" t="s">
         <v>372</v>
       </c>
@@ -12992,7 +12996,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="33" spans="4:9">
+    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D33" s="7" t="s">
         <v>369</v>
       </c>
@@ -13003,7 +13007,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="34" spans="4:9">
+    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D34" s="22" t="s">
         <v>366</v>
       </c>
@@ -13017,7 +13021,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="35" spans="4:9">
+    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D35" s="7" t="s">
         <v>364</v>
       </c>
@@ -13031,7 +13035,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="36" spans="4:9">
+    <row r="36" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D36" s="22" t="s">
         <v>361</v>
       </c>
@@ -13045,7 +13049,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="37" spans="4:9">
+    <row r="37" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D37" s="7" t="s">
         <v>359</v>
       </c>
@@ -13059,7 +13063,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="38" spans="4:9">
+    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>355</v>
       </c>
@@ -13067,7 +13071,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="39" spans="4:9">
+    <row r="39" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>354</v>
       </c>
@@ -13075,7 +13079,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="40" spans="4:9">
+    <row r="40" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>352</v>
       </c>
@@ -13086,7 +13090,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="41" spans="4:9">
+    <row r="41" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>350</v>
       </c>
@@ -13097,7 +13101,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="42" spans="4:9">
+    <row r="42" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D42" s="7" t="s">
         <v>347</v>
       </c>
@@ -13105,7 +13109,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="43" spans="4:9">
+    <row r="43" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>345</v>
       </c>
@@ -13113,7 +13117,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="44" spans="4:9">
+    <row r="44" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
         <v>344</v>
       </c>
@@ -13121,7 +13125,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="45" spans="4:9">
+    <row r="45" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
         <v>342</v>
       </c>
@@ -13129,7 +13133,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="46" spans="4:9">
+    <row r="46" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D46" s="7" t="s">
         <v>340</v>
       </c>
@@ -13137,7 +13141,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="47" spans="4:9">
+    <row r="47" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D47" s="7" t="s">
         <v>338</v>
       </c>
@@ -13145,7 +13149,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="48" spans="4:9">
+    <row r="48" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
         <v>337</v>
       </c>
@@ -13153,7 +13157,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="49" spans="4:7">
+    <row r="49" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
         <v>335</v>
       </c>
@@ -13161,7 +13165,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="54" spans="4:7">
+    <row r="54" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
         <v>334</v>
       </c>
@@ -13175,7 +13179,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="55" spans="4:7">
+    <row r="55" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
         <v>327</v>
       </c>
@@ -13189,7 +13193,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="56" spans="4:7">
+    <row r="56" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
         <v>325</v>
       </c>
@@ -13200,27 +13204,27 @@
         <v>326</v>
       </c>
     </row>
-    <row r="57" spans="4:7">
+    <row r="57" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="58" spans="4:7">
+    <row r="58" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="59" spans="4:7">
+    <row r="59" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="60" spans="4:7">
+    <row r="60" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="63" spans="4:7">
+    <row r="63" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
         <v>331</v>
       </c>
@@ -13231,7 +13235,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="64" spans="4:7">
+    <row r="64" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
         <v>328</v>
       </c>
@@ -13242,7 +13246,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="65" spans="4:6">
+    <row r="65" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
         <v>326</v>
       </c>
@@ -13253,7 +13257,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="66" spans="4:6">
+    <row r="66" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
         <v>321</v>
       </c>
@@ -13264,7 +13268,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="67" spans="4:6">
+    <row r="67" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E67" t="s">
         <v>323</v>
       </c>
@@ -13272,7 +13276,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="68" spans="4:6">
+    <row r="68" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E68" t="s">
         <v>322</v>
       </c>
@@ -13280,7 +13284,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="69" spans="4:6">
+    <row r="69" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E69" t="s">
         <v>321</v>
       </c>
@@ -13288,7 +13292,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="70" spans="4:6">
+    <row r="70" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E70" t="s">
         <v>320</v>
       </c>
@@ -13296,7 +13300,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="71" spans="4:6">
+    <row r="71" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E71" t="s">
         <v>319</v>
       </c>
@@ -13304,7 +13308,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="72" spans="4:6">
+    <row r="72" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F72" t="s">
         <v>318</v>
       </c>

</xml_diff>